<commit_message>
Refactoring of data: organized files into a better file structure and added alternate TestBase and config files per web site urls
</commit_message>
<xml_diff>
--- a/src/main/java/com/testdata/ExpressRegistrationTestdata2.xlsx
+++ b/src/main/java/com/testdata/ExpressRegistrationTestdata2.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="22">
   <si>
     <t xml:space="preserve">email</t>
   </si>
@@ -178,7 +178,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -192,6 +192,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -209,7 +210,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
@@ -218,6 +219,7 @@
   <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="6" max="6" bestFit="true" customWidth="true" width="6.3515625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="6.3515625" collapsed="true"/>
     <col min="1021" max="1025" customWidth="true" hidden="false" style="0" width="11.52" collapsed="true" outlineLevel="0"/>
   </cols>
   <sheetData>
@@ -240,6 +242,9 @@
       <c r="F1" t="s" s="3">
         <v>20</v>
       </c>
+      <c r="G1" t="s" s="4">
+        <v>20</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
@@ -260,6 +265,9 @@
       <c r="F2" t="s">
         <v>21</v>
       </c>
+      <c r="G2" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
@@ -280,6 +288,9 @@
       <c r="F3" t="s">
         <v>21</v>
       </c>
+      <c r="G3" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
@@ -298,6 +309,9 @@
         <v>19</v>
       </c>
       <c r="F4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" t="s">
         <v>21</v>
       </c>
     </row>

</xml_diff>